<commit_message>
consistent treatment of factors, fix q14 values
</commit_message>
<xml_diff>
--- a/data/lit_review_data_bjoern.xlsx
+++ b/data/lit_review_data_bjoern.xlsx
@@ -220,12 +220,6 @@
 	-Bjoern</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Z50">
-      <text>
-        <t xml:space="preserve">estimation and testing
-	-Bjoern</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="V100">
       <text>
         <t xml:space="preserve">between 60 and 480 items with one parameter each?
@@ -256,12 +250,6 @@
 	-Bjoern</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Z101">
-      <text>
-        <t xml:space="preserve">model selection, testing
-	-Bjoern</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="AM21">
       <text>
         <t xml:space="preserve">in the supplement
@@ -277,12 +265,6 @@
     <comment authorId="0" ref="L97">
       <text>
         <t xml:space="preserve">some were based on previous simulation study, some new
-	-Bjoern</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="Z102">
-      <text>
-        <t xml:space="preserve">estimation, testing
 	-Bjoern</t>
       </text>
     </comment>
@@ -328,12 +310,6 @@
 	-Bjoern</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Z91">
-      <text>
-        <t xml:space="preserve">estimation, model selection
-	-Bjoern</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="V84">
       <text>
         <t xml:space="preserve">really depends, again. It is an adaptive testing scheme with 600 items, but the number of estimated parameters of course depends on the adaptive test
@@ -349,12 +325,6 @@
     <comment authorId="0" ref="AL101">
       <text>
         <t xml:space="preserve">Monte Carlo SD, could be used to calculate SE. Also ANOVA
-	-Bjoern</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="Z5">
-      <text>
-        <t xml:space="preserve">and model selection
 	-Bjoern</t>
       </text>
     </comment>
@@ -430,12 +400,6 @@
 	-Bjoern</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Z98">
-      <text>
-        <t xml:space="preserve">estimation, classification
-	-Bjoern</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="X90">
       <text>
         <t xml:space="preserve">not sure here. The parameters are implied by the model, but does this make them known?
@@ -448,12 +412,6 @@
 	-Bjoern</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Z7">
-      <text>
-        <t xml:space="preserve">also estimation
-	-Bjoern</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="R99">
       <text>
         <t xml:space="preserve">it's a group-level model, so each dataset just once?
@@ -463,18 +421,6 @@
     <comment authorId="0" ref="W13">
       <text>
         <t xml:space="preserve">aggregated in figure
-	-Bjoern</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="Z29">
-      <text>
-        <t xml:space="preserve">estimation and testing
-	-Bjoern</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="Z90">
-      <text>
-        <t xml:space="preserve">estimation, testing
 	-Bjoern</t>
       </text>
     </comment>
@@ -495,7 +441,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="433">
   <si>
     <t>year</t>
   </si>
@@ -737,6 +683,9 @@
     <t>"We simulated a total of 50 samples for each condition; a number that is customary for simulation studies in Bayesian psychometrics because MCMC algorithms are very time-consuming. This number of samples is sufficient to estimate means and variances of the sampled quantities and to identify patterns in the data, while keeping computation within reasonable time limits (Levy et al., 2015)."</t>
   </si>
   <si>
+    <t>estimation, model selection</t>
+  </si>
+  <si>
     <t>EPR, EPS</t>
   </si>
   <si>
@@ -773,246 +722,249 @@
     <t>fully-factorial</t>
   </si>
   <si>
+    <t>design, estimation</t>
+  </si>
+  <si>
+    <t>median of quantiles of newly developed metric</t>
+  </si>
+  <si>
+    <t>Difference between certain quantiles of a metric and true parameter shown, could be seen as bias</t>
+  </si>
+  <si>
+    <t>unclear to me if the first simulation study of the paper is supposed to be a simulation study or just an example of simulation-based power analysis; kept very brief</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/00273171.2020.1809981</t>
+  </si>
+  <si>
+    <t>"three simulation studies were conducted to evaluate the performance of 15 statistics"</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>CCR (correct classifcation rate)</t>
+  </si>
+  <si>
+    <t>For some conditions, only "best" results are shown, other results are in the supplement</t>
+  </si>
+  <si>
+    <t>figures look like screenshots from an excel spreadsheet</t>
+  </si>
+  <si>
+    <t>great</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/00273171.2020.1815513</t>
+  </si>
+  <si>
+    <t>"Monte Carlo simulations were conducted to examine the finite-sample properties of the SEKF estimator in nonlinear time-varying parameter state space models." […] "in addition to the overall performance of the estimator in terms of parameter recovery we were also interested in answering a number of preliminary questions relevant to the use of these models in psychological research. First, is the estimator able to accurately recover multiple timevarying parameters when they exist in the data generating model? Second, what is the impact of allowing many model parameters to vary in the estimated model when only a subset of those parameters are time-varying in the true or data generating model? Finally, we also wanted to better understand the potential advantages of our proposed square-root algorithm (SR-SEKF) over the standard second-order EKF (SEKF)."</t>
+  </si>
+  <si>
+    <t>two different scenarios as main conditions</t>
+  </si>
+  <si>
+    <t>4+</t>
+  </si>
+  <si>
+    <t>efficiency (standard deviation of estimates), accuracy, computational efficiency (number of iterations)</t>
+  </si>
+  <si>
+    <t>they use the mean percentage of relative bias as performance measure, with no decimal places. Seems a bit misleading</t>
+  </si>
+  <si>
+    <t>"All the estimation routines described in this paper and employed for the simulations and empirical example were coded in R by the first author."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">they call it two simulations, but later state that these are the two "main simulation conditions". I've coded it as one sim. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.1037/met0000444 </t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>A simulation study was designed to answer the following questions when the same conditions of the empirical study (i.e., the same number of time points, trials, persons, items, and sessions) and covariates are considered: (a) can the fixed experimental condition effects and their standard errors be recovered?; (b) what are the consequences of ignoring spatial and temporal effects in testing the experimental condition effects?</t>
+  </si>
+  <si>
+    <t>parametric based on actual data</t>
+  </si>
+  <si>
+    <t>simulate from estimated model, then compare two modelling strategies</t>
+  </si>
+  <si>
+    <t>estimated</t>
+  </si>
+  <si>
+    <t>standard deviations</t>
+  </si>
+  <si>
+    <t>they merely implemented it in mgcv</t>
+  </si>
+  <si>
+    <t>they provide extensive code for model fitting, which also includes a seed somewhere. But they do not provide the code for their simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.1037/met0000359 </t>
+  </si>
+  <si>
+    <t>"Although the validity of our sampling algorithm can be justified on mathematical grounds (Geman and Geman, 1984), in this section we provide a simulation to further demonstrate the model performance and its ability to generate a rich set of output."</t>
+  </si>
+  <si>
+    <t>they look at difference between estimate and true value and at Credible Interval, but they do not calculate a performance measure</t>
+  </si>
+  <si>
+    <t>R, Stata</t>
+  </si>
+  <si>
+    <t>"The R code and data used in this paper are available in GitHub at https:// github.com/jtm508/bayestraj. Vignettes are also provided to help users adapt the code to applications of their own interest."</t>
+  </si>
+  <si>
+    <t>accessible online</t>
+  </si>
+  <si>
+    <t>https://github.com/jtm508/bayestraj</t>
+  </si>
+  <si>
+    <t>not sure if this should be included. More of a demonstration than a full simulation</t>
+  </si>
+  <si>
+    <t>http://doi.org/10.1037/met0000368</t>
+  </si>
+  <si>
+    <t>"We conducted two simulation studies to determine how well our latent mixture-based method performs compared with the traditional methods. The simulation studies focused on two outcomes. One was the comparison of statistical power (i.e., 1 _x0004_ Type II error rate) attained by different methods given the same Type I error rate."</t>
+  </si>
+  <si>
+    <t>did not vary low level of moderator (give a long explanation for that)</t>
+  </si>
+  <si>
+    <t>No information on this anywhere</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>"The download link and a brief description of an R package for our latent mixture-based method is available in the online supplemental materials."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.1037/met0000387 </t>
+  </si>
+  <si>
+    <t>"systemically examine the effectivesness of the Bayesian Lasso in three factor loading settings:[…]"</t>
+  </si>
+  <si>
+    <t>more of parameter recovery study than full simulation</t>
+  </si>
+  <si>
+    <t>Sounds like they just simulated data without repeated iterations</t>
+  </si>
+  <si>
+    <t>384+?</t>
+  </si>
+  <si>
+    <t>correlation estimated with true values, false-alarm rate, miss rate</t>
+  </si>
+  <si>
+    <t>they talk about bias in the results, but do not actually compute it; only look at it visually</t>
+  </si>
+  <si>
+    <t>wrote their own MCMC sampler</t>
+  </si>
+  <si>
+    <t>https://github.com/MbCN-lab/LassoFANDDM</t>
+  </si>
+  <si>
+    <t>seed is not in the simulation script, but in the "main" script. Still counted it as yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.1037/met0000351 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.1037/met0000408 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.1037/met0000415 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://doi.org/10.1037/met0000505 </t>
+  </si>
+  <si>
+    <t>http://doi.org/10.1037/met0000319</t>
+  </si>
+  <si>
+    <t>"to compare this implementation with three other maximum likelihood-based models in their accuracy to estimate true scores"</t>
+  </si>
+  <si>
+    <t>sample size, dgp</t>
+  </si>
+  <si>
+    <t>MAE, correlation between estimates and true values</t>
+  </si>
+  <si>
+    <t>R, JAGS</t>
+  </si>
+  <si>
+    <t>JAGS model</t>
+  </si>
+  <si>
+    <t>https://osf.io/5vnxc/</t>
+  </si>
+  <si>
+    <t>seed provided in a different part of the scripts, but still coded as "yes"</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/met0000312</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/met0000314</t>
+  </si>
+  <si>
+    <t>"Three simulation studies were conducted to illustrate estimating the proposed interventional indirect effects. […] simply to demonstrate the estimators presented in the preceding section"</t>
+  </si>
+  <si>
+    <t>sample size</t>
+  </si>
+  <si>
+    <t>they check if average estimate is equal to true coefficient, which could be interpreted as bias</t>
+  </si>
+  <si>
+    <t>https://github.com/wwloh/disentangle-multiple-mediators</t>
+  </si>
+  <si>
+    <t>the simulation coded here merely dealt as illustration that a certain model specification can recover unbiased estimates on average</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/met0000340</t>
+  </si>
+  <si>
+    <t>"we run simulations to assess, if all the functional and distributional assumptions of the mediator and outcome are satisfied or if part of them is violated, to what extent the proposed sensitivity analysis strategy would approximate the true NIE and NDE when incorporated with the regression-based and weighting-based causal mediation analysis methods"</t>
+  </si>
+  <si>
+    <t>model specification, link function, error distribution, type of misspecification, sensitivity parameters</t>
+  </si>
+  <si>
+    <t>visual inspection of median estimate with true estimate (no calculation), sampling variability (visual inspection of boxplot)</t>
+  </si>
+  <si>
+    <t>We have also developed an R package that implements the proposed method (https://cran.r-project.org/web/packages/mediationsens/index.html).</t>
+  </si>
+  <si>
+    <t>this was the most unneccessarily complex description of a simulation study so far. Different subscenarios within different scenarios</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/met0000330</t>
+  </si>
+  <si>
+    <t>"we evaluate the robustness of the proposed power analysis by focusing on the two assumptions—constant within-cluster variance of predictor and constant cluster size"</t>
+  </si>
+  <si>
+    <t>L2 sample size, cluster size, data-generating mechanism, effect in focus</t>
+  </si>
+  <si>
     <t>design</t>
   </si>
   <si>
-    <t>median of quantiles of newly developed metric</t>
-  </si>
-  <si>
-    <t>Difference between certain quantiles of a metric and true parameter shown, could be seen as bias</t>
-  </si>
-  <si>
-    <t>unclear to me if the first simulation study of the paper is supposed to be a simulation study or just an example of simulation-based power analysis; kept very brief</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1080/00273171.2020.1809981</t>
-  </si>
-  <si>
-    <t>"three simulation studies were conducted to evaluate the performance of 15 statistics"</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>CCR (correct classifcation rate)</t>
-  </si>
-  <si>
-    <t>For some conditions, only "best" results are shown, other results are in the supplement</t>
-  </si>
-  <si>
-    <t>figures look like screenshots from an excel spreadsheet</t>
-  </si>
-  <si>
-    <t>great</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1080/00273171.2020.1815513</t>
-  </si>
-  <si>
-    <t>"Monte Carlo simulations were conducted to examine the finite-sample properties of the SEKF estimator in nonlinear time-varying parameter state space models." […] "in addition to the overall performance of the estimator in terms of parameter recovery we were also interested in answering a number of preliminary questions relevant to the use of these models in psychological research. First, is the estimator able to accurately recover multiple timevarying parameters when they exist in the data generating model? Second, what is the impact of allowing many model parameters to vary in the estimated model when only a subset of those parameters are time-varying in the true or data generating model? Finally, we also wanted to better understand the potential advantages of our proposed square-root algorithm (SR-SEKF) over the standard second-order EKF (SEKF)."</t>
-  </si>
-  <si>
-    <t>two different scenarios as main conditions</t>
-  </si>
-  <si>
-    <t>4+</t>
-  </si>
-  <si>
-    <t>efficiency (standard deviation of estimates), accuracy, computational efficiency (number of iterations)</t>
-  </si>
-  <si>
-    <t>they use the mean percentage of relative bias as performance measure, with no decimal places. Seems a bit misleading</t>
-  </si>
-  <si>
-    <t>"All the estimation routines described in this paper and employed for the simulations and empirical example were coded in R by the first author."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">they call it two simulations, but later state that these are the two "main simulation conditions". I've coded it as one sim. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://doi.org/10.1037/met0000444 </t>
-  </si>
-  <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <t>A simulation study was designed to answer the following questions when the same conditions of the empirical study (i.e., the same number of time points, trials, persons, items, and sessions) and covariates are considered: (a) can the fixed experimental condition effects and their standard errors be recovered?; (b) what are the consequences of ignoring spatial and temporal effects in testing the experimental condition effects?</t>
-  </si>
-  <si>
-    <t>parametric based on actual data</t>
-  </si>
-  <si>
-    <t>simulate from estimated model, then compare two modelling strategies</t>
-  </si>
-  <si>
-    <t>estimated</t>
-  </si>
-  <si>
-    <t>standard deviations</t>
-  </si>
-  <si>
-    <t>they merely implemented it in mgcv</t>
-  </si>
-  <si>
-    <t>they provide extensive code for model fitting, which also includes a seed somewhere. But they do not provide the code for their simulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://doi.org/10.1037/met0000359 </t>
-  </si>
-  <si>
-    <t>"Although the validity of our sampling algorithm can be justified on mathematical grounds (Geman and Geman, 1984), in this section we provide a simulation to further demonstrate the model performance and its ability to generate a rich set of output."</t>
-  </si>
-  <si>
-    <t>they look at difference between estimate and true value and at Credible Interval, but they do not calculate a performance measure</t>
-  </si>
-  <si>
-    <t>R, Stata</t>
-  </si>
-  <si>
-    <t>"The R code and data used in this paper are available in GitHub at https:// github.com/jtm508/bayestraj. Vignettes are also provided to help users adapt the code to applications of their own interest."</t>
-  </si>
-  <si>
-    <t>accessible online</t>
-  </si>
-  <si>
-    <t>https://github.com/jtm508/bayestraj</t>
-  </si>
-  <si>
-    <t>not sure if this should be included. More of a demonstration than a full simulation</t>
-  </si>
-  <si>
-    <t>http://doi.org/10.1037/met0000368</t>
-  </si>
-  <si>
-    <t>"We conducted two simulation studies to determine how well our latent mixture-based method performs compared with the traditional methods. The simulation studies focused on two outcomes. One was the comparison of statistical power (i.e., 1 _x0004_ Type II error rate) attained by different methods given the same Type I error rate."</t>
-  </si>
-  <si>
-    <t>did not vary low level of moderator (give a long explanation for that)</t>
-  </si>
-  <si>
-    <t>No information on this anywhere</t>
-  </si>
-  <si>
-    <t>table</t>
-  </si>
-  <si>
-    <t>"The download link and a brief description of an R package for our latent mixture-based method is available in the online supplemental materials."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://doi.org/10.1037/met0000387 </t>
-  </si>
-  <si>
-    <t>"systemically examine the effectivesness of the Bayesian Lasso in three factor loading settings:[…]"</t>
-  </si>
-  <si>
-    <t>more of parameter recovery study than full simulation</t>
-  </si>
-  <si>
-    <t>Sounds like they just simulated data without repeated iterations</t>
-  </si>
-  <si>
-    <t>384+?</t>
-  </si>
-  <si>
-    <t>correlation estimated with true values, false-alarm rate, miss rate</t>
-  </si>
-  <si>
-    <t>they talk about bias in the results, but do not actually compute it; only look at it visually</t>
-  </si>
-  <si>
-    <t>wrote their own MCMC sampler</t>
-  </si>
-  <si>
-    <t>https://github.com/MbCN-lab/LassoFANDDM</t>
-  </si>
-  <si>
-    <t>seed is not in the simulation script, but in the "main" script. Still counted it as yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://doi.org/10.1037/met0000351 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://doi.org/10.1037/met0000408 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://doi.org/10.1037/met0000415 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://doi.org/10.1037/met0000505 </t>
-  </si>
-  <si>
-    <t>http://doi.org/10.1037/met0000319</t>
-  </si>
-  <si>
-    <t>"to compare this implementation with three other maximum likelihood-based models in their accuracy to estimate true scores"</t>
-  </si>
-  <si>
-    <t>sample size, dgp</t>
-  </si>
-  <si>
-    <t>MAE, correlation between estimates and true values</t>
-  </si>
-  <si>
-    <t>R, JAGS</t>
-  </si>
-  <si>
-    <t>JAGS model</t>
-  </si>
-  <si>
-    <t>https://osf.io/5vnxc/</t>
-  </si>
-  <si>
-    <t>seed provided in a different part of the scripts, but still coded as "yes"</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1037/met0000312</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1037/met0000314</t>
-  </si>
-  <si>
-    <t>"Three simulation studies were conducted to illustrate estimating the proposed interventional indirect effects. […] simply to demonstrate the estimators presented in the preceding section"</t>
-  </si>
-  <si>
-    <t>sample size</t>
-  </si>
-  <si>
-    <t>they check if average estimate is equal to true coefficient, which could be interpreted as bias</t>
-  </si>
-  <si>
-    <t>https://github.com/wwloh/disentangle-multiple-mediators</t>
-  </si>
-  <si>
-    <t>the simulation coded here merely dealt as illustration that a certain model specification can recover unbiased estimates on average</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1037/met0000340</t>
-  </si>
-  <si>
-    <t>"we run simulations to assess, if all the functional and distributional assumptions of the mediator and outcome are satisfied or if part of them is violated, to what extent the proposed sensitivity analysis strategy would approximate the true NIE and NDE when incorporated with the regression-based and weighting-based causal mediation analysis methods"</t>
-  </si>
-  <si>
-    <t>model specification, link function, error distribution, type of misspecification, sensitivity parameters</t>
-  </si>
-  <si>
-    <t>visual inspection of median estimate with true estimate (no calculation), sampling variability (visual inspection of boxplot)</t>
-  </si>
-  <si>
-    <t>We have also developed an R package that implements the proposed method (https://cran.r-project.org/web/packages/mediationsens/index.html).</t>
-  </si>
-  <si>
-    <t>this was the most unneccessarily complex description of a simulation study so far. Different subscenarios within different scenarios</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1037/met0000330</t>
-  </si>
-  <si>
-    <t>"we evaluate the robustness of the proposed power analysis by focusing on the two assumptions—constant within-cluster variance of predictor and constant cluster size"</t>
-  </si>
-  <si>
-    <t>L2 sample size, cluster size, data-generating mechanism, effect in focus</t>
-  </si>
-  <si>
     <t>RMSE of the power compared to another power analysis method</t>
   </si>
   <si>
@@ -1082,6 +1034,9 @@
     <t>"A simulation study was conducted to (i) compare the performance of the 2moME model against that of the conventional moME model, and (ii) examine the performance of Bayesian methods in estimating and testing the moME effects and the corresponding ESs under different conditions."</t>
   </si>
   <si>
+    <t>estimation, testing</t>
+  </si>
+  <si>
     <t>extensive supplement containing all results</t>
   </si>
   <si>
@@ -1679,6 +1634,9 @@
     <t>7+</t>
   </si>
   <si>
+    <t>estimation, classification</t>
+  </si>
+  <si>
     <t>pattern correct classification rate, attribute correct clasisification rate</t>
   </si>
   <si>
@@ -1743,6 +1701,9 @@
   </si>
   <si>
     <t>sample size, model size, factor loading level, factor inter-correlations</t>
+  </si>
+  <si>
+    <t>model selection, testing</t>
   </si>
   <si>
     <t>proportion of model fit rejection, means and standard deviations of estimates, coefficient of variation</t>
@@ -1876,11 +1837,11 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2241,7 +2202,7 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
@@ -2688,8 +2649,8 @@
       <c r="Y5" s="1">
         <v>2.0</v>
       </c>
-      <c r="Z5" s="1" t="s">
-        <v>66</v>
+      <c r="Z5" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>56</v>
@@ -2716,16 +2677,16 @@
         <v>56</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ5" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AM5" s="1" t="s">
         <v>58</v>
@@ -2740,7 +2701,7 @@
         <v>56</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AR5" s="1" t="s">
         <v>56</v>
@@ -2760,13 +2721,13 @@
         <v>56</v>
       </c>
       <c r="AY5" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AZ5" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="BA5" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB5" s="3">
         <v>45083.0</v>
@@ -2783,7 +2744,7 @@
         <v>1.0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>54</v>
@@ -2853,7 +2814,7 @@
         <v>1.0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>54</v>
@@ -2874,7 +2835,7 @@
         <v>58</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>60</v>
@@ -2886,13 +2847,13 @@
         <v>6.0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P7" s="1">
         <v>1.0</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R7" s="1">
         <v>10.0</v>
@@ -2916,8 +2877,8 @@
       <c r="Y7" s="1">
         <v>1.0</v>
       </c>
-      <c r="Z7" s="1" t="s">
-        <v>92</v>
+      <c r="Z7" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>56</v>
@@ -2944,13 +2905,13 @@
         <v>56</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ7" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AL7" s="1" t="s">
         <v>67</v>
@@ -2989,10 +2950,10 @@
       </c>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA7" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB7" s="3">
         <v>45083.0</v>
@@ -3009,7 +2970,7 @@
         <v>1.0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>54</v>
@@ -3030,7 +2991,7 @@
         <v>58</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>60</v>
@@ -3046,7 +3007,7 @@
         <v>3.0</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R8" s="1">
         <v>200.0</v>
@@ -3071,7 +3032,7 @@
         <v>1.0</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>56</v>
@@ -3098,13 +3059,13 @@
         <v>56</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AJ8" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK8" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AL8" s="1" t="s">
         <v>67</v>
@@ -3142,10 +3103,10 @@
         <v>56</v>
       </c>
       <c r="AZ8" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="BA8" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB8" s="3">
         <v>45084.0</v>
@@ -3162,7 +3123,7 @@
         <v>1.0</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>54</v>
@@ -3183,7 +3144,7 @@
         <v>58</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>60</v>
@@ -3195,13 +3156,13 @@
         <v>12.0</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P9" s="1">
         <v>3.0</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R9" s="1">
         <v>100.0</v>
@@ -3214,7 +3175,7 @@
         <v>58</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>56</v>
@@ -3253,13 +3214,13 @@
         <v>56</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AJ9" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK9" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AL9" s="1" t="s">
         <v>67</v>
@@ -3283,7 +3244,7 @@
         <v>58</v>
       </c>
       <c r="AS9" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AT9" s="1" t="s">
         <v>70</v>
@@ -3300,10 +3261,10 @@
       </c>
       <c r="AY9" s="1"/>
       <c r="AZ9" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="BA9" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB9" s="3">
         <v>45084.0</v>
@@ -3320,10 +3281,10 @@
         <v>3.0</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>55</v>
@@ -3341,10 +3302,10 @@
         <v>58</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>58</v>
@@ -3353,7 +3314,7 @@
         <v>1.0</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P10" s="1">
         <v>0.0</v>
@@ -3378,7 +3339,7 @@
         <v>58</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Y10" s="1">
         <v>2.0</v>
@@ -3411,7 +3372,7 @@
         <v>56</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
@@ -3437,7 +3398,7 @@
         <v>56</v>
       </c>
       <c r="AS10" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AT10" s="1" t="s">
         <v>70</v>
@@ -3453,11 +3414,11 @@
         <v>56</v>
       </c>
       <c r="AY10" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AZ10" s="1"/>
       <c r="BA10" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB10" s="3">
         <v>45090.0</v>
@@ -3474,10 +3435,10 @@
         <v>3.0</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>55</v>
@@ -3495,7 +3456,7 @@
         <v>58</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>60</v>
@@ -3567,7 +3528,7 @@
         <v>56</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AL11" s="1" t="s">
         <v>67</v>
@@ -3585,19 +3546,19 @@
         <v>56</v>
       </c>
       <c r="AQ11" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AR11" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AS11" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AT11" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU11" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AV11" s="1" t="s">
         <v>58</v>
@@ -3610,10 +3571,10 @@
       </c>
       <c r="AY11" s="1"/>
       <c r="AZ11" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="BA11" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB11" s="3">
         <v>45090.0</v>
@@ -3630,10 +3591,10 @@
         <v>3.0</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>55</v>
@@ -3651,7 +3612,7 @@
         <v>58</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>60</v>
@@ -3663,7 +3624,7 @@
         <v>108.0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P12" s="1">
         <v>4.0</v>
@@ -3678,7 +3639,7 @@
         <v>56</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>58</v>
@@ -3696,7 +3657,7 @@
         <v>3.0</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AA12" s="1" t="s">
         <v>56</v>
@@ -3723,14 +3684,14 @@
         <v>56</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AJ12" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK12" s="1"/>
       <c r="AL12" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM12" s="1" t="s">
         <v>56</v>
@@ -3751,7 +3712,7 @@
         <v>58</v>
       </c>
       <c r="AS12" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AT12" s="1" t="s">
         <v>70</v>
@@ -3769,7 +3730,7 @@
       <c r="AY12" s="1"/>
       <c r="AZ12" s="1"/>
       <c r="BA12" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB12" s="3">
         <v>45090.0</v>
@@ -3786,10 +3747,10 @@
         <v>3.0</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>55</v>
@@ -3807,7 +3768,7 @@
         <v>58</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>60</v>
@@ -3819,7 +3780,7 @@
         <v>1.0</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="P13" s="1">
         <v>0.0</v>
@@ -3834,13 +3795,13 @@
         <v>56</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>56</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>58</v>
@@ -3879,13 +3840,13 @@
         <v>56</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AJ13" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AL13" s="1" t="s">
         <v>67</v>
@@ -3909,13 +3870,13 @@
         <v>58</v>
       </c>
       <c r="AS13" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AT13" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU13" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AV13" s="1" t="s">
         <v>58</v>
@@ -3927,13 +3888,13 @@
         <v>56</v>
       </c>
       <c r="AY13" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AZ13" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="BA13" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB13" s="3">
         <v>45103.0</v>
@@ -3950,10 +3911,10 @@
         <v>3.0</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>55</v>
@@ -4020,10 +3981,10 @@
         <v>3.0</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
@@ -4090,10 +4051,10 @@
         <v>3.0</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>55</v>
@@ -4160,10 +4121,10 @@
         <v>3.0</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>55</v>
@@ -4230,10 +4191,10 @@
         <v>6.0</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>55</v>
@@ -4251,7 +4212,7 @@
         <v>58</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>60</v>
@@ -4263,13 +4224,13 @@
         <v>9.0</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="P18" s="1">
         <v>2.0</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R18" s="1">
         <v>100.0</v>
@@ -4321,7 +4282,7 @@
         <v>58</v>
       </c>
       <c r="AI18" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AJ18" s="1" t="s">
         <v>58</v>
@@ -4343,19 +4304,19 @@
         <v>56</v>
       </c>
       <c r="AQ18" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AR18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AS18" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AT18" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU18" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AV18" s="1" t="s">
         <v>58</v>
@@ -4367,11 +4328,11 @@
         <v>56</v>
       </c>
       <c r="AY18" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AZ18" s="1"/>
       <c r="BA18" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB18" s="3">
         <v>45101.0</v>
@@ -4388,10 +4349,10 @@
         <v>6.0</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>55</v>
@@ -4458,10 +4419,10 @@
         <v>6.0</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>55</v>
@@ -4479,10 +4440,10 @@
         <v>58</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>58</v>
@@ -4491,13 +4452,13 @@
         <v>3.0</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P20" s="1">
         <v>1.0</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R20" s="1">
         <v>10000.0</v>
@@ -4553,7 +4514,7 @@
         <v>58</v>
       </c>
       <c r="AK20" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AL20" s="1" t="s">
         <v>67</v>
@@ -4578,10 +4539,10 @@
       </c>
       <c r="AS20" s="1"/>
       <c r="AT20" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU20" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AV20" s="1"/>
       <c r="AW20" s="1" t="s">
@@ -4592,10 +4553,10 @@
       </c>
       <c r="AY20" s="1"/>
       <c r="AZ20" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BA20" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB20" s="3">
         <v>45101.0</v>
@@ -4612,10 +4573,10 @@
         <v>6.0</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>55</v>
@@ -4633,7 +4594,7 @@
         <v>58</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>60</v>
@@ -4645,7 +4606,7 @@
         <v>102.0</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P21" s="1">
         <v>5.0</v>
@@ -4703,14 +4664,14 @@
         <v>56</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AJ21" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AM21" s="1" t="s">
         <v>58</v>
@@ -4731,7 +4692,7 @@
         <v>58</v>
       </c>
       <c r="AS21" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AT21" s="1" t="s">
         <v>70</v>
@@ -4746,10 +4707,10 @@
       </c>
       <c r="AY21" s="1"/>
       <c r="AZ21" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="BA21" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB21" s="3">
         <v>45103.0</v>
@@ -4766,10 +4727,10 @@
         <v>6.0</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>55</v>
@@ -4787,7 +4748,7 @@
         <v>58</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>60</v>
@@ -4799,13 +4760,13 @@
         <v>81.0</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="P22" s="1">
         <v>2.0</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R22" s="1">
         <v>500.0</v>
@@ -4830,7 +4791,7 @@
         <v>3.0</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>92</v>
+        <v>173</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>56</v>
@@ -4861,10 +4822,10 @@
         <v>58</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AL22" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AM22" s="1" t="s">
         <v>56</v>
@@ -4885,7 +4846,7 @@
         <v>58</v>
       </c>
       <c r="AS22" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AT22" s="1" t="s">
         <v>70</v>
@@ -4899,11 +4860,11 @@
         <v>56</v>
       </c>
       <c r="AY22" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AZ22" s="1"/>
       <c r="BA22" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB22" s="3">
         <v>45103.0</v>
@@ -4920,10 +4881,10 @@
         <v>6.0</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
@@ -4990,10 +4951,10 @@
         <v>6.0</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>55</v>
@@ -5046,7 +5007,7 @@
       <c r="AX24" s="1"/>
       <c r="AY24" s="1"/>
       <c r="AZ24" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="BA24" s="1"/>
       <c r="BB24" s="3"/>
@@ -5061,11 +5022,11 @@
       <c r="C25" s="1">
         <v>6.0</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>179</v>
+      <c r="D25" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>55</v>
@@ -5083,17 +5044,19 @@
         <v>58</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M25" s="1"/>
+      <c r="M25" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="N25" s="1">
         <v>1296.0</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="P25" s="1">
         <v>7.0</v>
@@ -5108,7 +5071,7 @@
         <v>58</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>58</v>
@@ -5153,14 +5116,14 @@
         <v>56</v>
       </c>
       <c r="AI25" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AJ25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AM25" s="1" t="s">
         <v>58</v>
@@ -5175,19 +5138,19 @@
         <v>56</v>
       </c>
       <c r="AQ25" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AR25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AT25" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU25" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AV25" s="1" t="s">
         <v>71</v>
@@ -5199,11 +5162,11 @@
         <v>56</v>
       </c>
       <c r="AY25" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AZ25" s="1"/>
       <c r="BA25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB25" s="3">
         <v>45103.0</v>
@@ -5220,10 +5183,10 @@
         <v>6.0</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>55</v>
@@ -5276,7 +5239,7 @@
       <c r="AX26" s="1"/>
       <c r="AY26" s="1"/>
       <c r="AZ26" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="BA26" s="1"/>
       <c r="BB26" s="3"/>
@@ -5292,10 +5255,10 @@
         <v>2.0</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>55</v>
@@ -5362,10 +5325,10 @@
         <v>2.0</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>55</v>
@@ -5416,7 +5379,7 @@
       <c r="AX28" s="1"/>
       <c r="AY28" s="1"/>
       <c r="AZ28" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="BA28" s="1"/>
       <c r="BB28" s="3"/>
@@ -5432,10 +5395,10 @@
         <v>2.0</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>55</v>
@@ -5453,7 +5416,7 @@
         <v>58</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>60</v>
@@ -5469,7 +5432,7 @@
         <v>3.0</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R29" s="1">
         <v>1000.0</v>
@@ -5493,8 +5456,8 @@
       <c r="Y29" s="1">
         <v>2.0</v>
       </c>
-      <c r="Z29" s="1" t="s">
-        <v>66</v>
+      <c r="Z29" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="AA29" s="1" t="s">
         <v>56</v>
@@ -5525,7 +5488,7 @@
         <v>58</v>
       </c>
       <c r="AK29" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AL29" s="1" t="s">
         <v>67</v>
@@ -5543,13 +5506,13 @@
         <v>56</v>
       </c>
       <c r="AQ29" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="AR29" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AS29" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AT29" s="1" t="s">
         <v>70</v>
@@ -5565,13 +5528,13 @@
         <v>56</v>
       </c>
       <c r="AY29" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="AZ29" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BA29" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB29" s="3">
         <v>45103.0</v>
@@ -5588,10 +5551,10 @@
         <v>2.0</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>55</v>
@@ -5658,10 +5621,10 @@
         <v>2.0</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>55</v>
@@ -5728,10 +5691,10 @@
         <v>2.0</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>55</v>
@@ -5798,10 +5761,10 @@
         <v>2.0</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>55</v>
@@ -5868,10 +5831,10 @@
         <v>2.0</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>55</v>
@@ -5938,10 +5901,10 @@
         <v>2.0</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>55</v>
@@ -6008,10 +5971,10 @@
         <v>2.0</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>55</v>
@@ -6078,10 +6041,10 @@
         <v>2.0</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>55</v>
@@ -6148,10 +6111,10 @@
         <v>2.0</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>55</v>
@@ -6218,10 +6181,10 @@
         <v>2.0</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>55</v>
@@ -6288,10 +6251,10 @@
         <v>2.0</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>55</v>
@@ -6358,10 +6321,10 @@
         <v>2.0</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>55</v>
@@ -6428,10 +6391,10 @@
         <v>2.0</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>55</v>
@@ -6449,10 +6412,10 @@
         <v>58</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>58</v>
@@ -6461,13 +6424,13 @@
         <v>8.0</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="P42" s="1">
         <v>3.0</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R42" s="1">
         <v>500.0</v>
@@ -6492,7 +6455,7 @@
         <v>2.0</v>
       </c>
       <c r="Z42" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="AA42" s="1" t="s">
         <v>56</v>
@@ -6519,13 +6482,13 @@
         <v>56</v>
       </c>
       <c r="AI42" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="AJ42" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK42" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="AL42" s="1" t="s">
         <v>67</v>
@@ -6550,10 +6513,10 @@
       </c>
       <c r="AS42" s="1"/>
       <c r="AT42" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU42" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AV42" s="1" t="s">
         <v>58</v>
@@ -6565,15 +6528,15 @@
         <v>56</v>
       </c>
       <c r="AY42" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="AZ42" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="BA42" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BB42" s="8">
+        <v>87</v>
+      </c>
+      <c r="BB42" s="9">
         <v>45099.0</v>
       </c>
     </row>
@@ -6588,10 +6551,10 @@
         <v>2.0</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>55</v>
@@ -6658,10 +6621,10 @@
         <v>2.0</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>55</v>
@@ -6728,10 +6691,10 @@
         <v>2.0</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>55</v>
@@ -6798,10 +6761,10 @@
         <v>2.0</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>55</v>
@@ -6868,10 +6831,10 @@
         <v>2.0</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>55</v>
@@ -6938,10 +6901,10 @@
         <v>2.0</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>55</v>
@@ -7008,10 +6971,10 @@
         <v>2.0</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>55</v>
@@ -7078,10 +7041,10 @@
         <v>2.0</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>55</v>
@@ -7099,7 +7062,7 @@
         <v>58</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>60</v>
@@ -7111,13 +7074,13 @@
         <v>1944.0</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="P50" s="1">
         <v>7.0</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R50" s="1">
         <v>1000.0</v>
@@ -7141,8 +7104,8 @@
       <c r="Y50" s="1">
         <v>1.0</v>
       </c>
-      <c r="Z50" s="1" t="s">
-        <v>66</v>
+      <c r="Z50" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="AA50" s="1" t="s">
         <v>56</v>
@@ -7173,7 +7136,7 @@
         <v>58</v>
       </c>
       <c r="AK50" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AL50" s="1" t="s">
         <v>67</v>
@@ -7191,19 +7154,19 @@
         <v>56</v>
       </c>
       <c r="AQ50" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AR50" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AS50" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AT50" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU50" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AV50" s="1" t="s">
         <v>58</v>
@@ -7215,13 +7178,13 @@
         <v>56</v>
       </c>
       <c r="AY50" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AZ50" s="1"/>
       <c r="BA50" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BB50" s="8">
+        <v>103</v>
+      </c>
+      <c r="BB50" s="9">
         <v>45099.0</v>
       </c>
     </row>
@@ -7236,10 +7199,10 @@
         <v>2.0</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>55</v>
@@ -7306,10 +7269,10 @@
         <v>2.0</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>55</v>
@@ -7376,10 +7339,10 @@
         <v>2.0</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>55</v>
@@ -7446,10 +7409,10 @@
         <v>2.0</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>55</v>
@@ -7516,10 +7479,10 @@
         <v>2.0</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>55</v>
@@ -7537,7 +7500,7 @@
         <v>56</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>60</v>
@@ -7549,13 +7512,13 @@
         <v>2.0</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="P55" s="1">
         <v>3.0</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R55" s="1">
         <v>100.0</v>
@@ -7627,19 +7590,19 @@
         <v>56</v>
       </c>
       <c r="AQ55" s="2" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="AR55" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AS55" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="AT55" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU55" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="AV55" s="1" t="s">
         <v>71</v>
@@ -7652,10 +7615,10 @@
       </c>
       <c r="AY55" s="1"/>
       <c r="AZ55" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="BA55" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB55" s="3">
         <v>45100.0</v>
@@ -7672,10 +7635,10 @@
         <v>2.0</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>55</v>
@@ -7742,10 +7705,10 @@
         <v>5.0</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>55</v>
@@ -7763,7 +7726,7 @@
         <v>58</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>60</v>
@@ -7775,13 +7738,13 @@
         <v>12.0</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="P57" s="1">
         <v>2.0</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R57" s="1">
         <v>500.0</v>
@@ -7794,7 +7757,7 @@
         <v>56</v>
       </c>
       <c r="V57" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>58</v>
@@ -7833,7 +7796,7 @@
         <v>56</v>
       </c>
       <c r="AI57" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="AJ57" s="1" t="s">
         <v>58</v>
@@ -7861,31 +7824,31 @@
         <v>58</v>
       </c>
       <c r="AS57" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="AT57" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU57" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="AV57" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AW57" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX57" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AY57" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="AZ57" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="BA57" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB57" s="3">
         <v>45100.0</v>
@@ -7901,11 +7864,11 @@
       <c r="C58" s="1">
         <v>5.0</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>258</v>
+      <c r="D58" s="8" t="s">
+        <v>261</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>55</v>
@@ -7972,10 +7935,10 @@
         <v>5.0</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>55</v>
@@ -7993,7 +7956,7 @@
         <v>58</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>60</v>
@@ -8005,13 +7968,13 @@
         <v>8.0</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="P59" s="1">
         <v>3.0</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R59" s="1">
         <v>500.0</v>
@@ -8024,7 +7987,7 @@
         <v>58</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>58</v>
@@ -8036,7 +7999,7 @@
         <v>3.0</v>
       </c>
       <c r="Z59" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AA59" s="1" t="s">
         <v>58</v>
@@ -8090,10 +8053,10 @@
       </c>
       <c r="AS59" s="1"/>
       <c r="AT59" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU59" s="5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="AV59" s="1" t="s">
         <v>58</v>
@@ -8105,13 +8068,13 @@
         <v>56</v>
       </c>
       <c r="AY59" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="AZ59" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="BA59" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB59" s="3">
         <v>45101.0</v>
@@ -8127,11 +8090,11 @@
       <c r="C60" s="1">
         <v>5.0</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>266</v>
+      <c r="D60" s="8" t="s">
+        <v>269</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>55</v>
@@ -8197,11 +8160,11 @@
       <c r="C61" s="1">
         <v>5.0</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>267</v>
+      <c r="D61" s="8" t="s">
+        <v>270</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>55</v>
@@ -8254,7 +8217,7 @@
       <c r="AX61" s="1"/>
       <c r="AY61" s="1"/>
       <c r="AZ61" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="BA61" s="1"/>
     </row>
@@ -8268,11 +8231,11 @@
       <c r="C62" s="1">
         <v>5.0</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>269</v>
+      <c r="D62" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>55</v>
@@ -8338,11 +8301,11 @@
       <c r="C63" s="1">
         <v>5.0</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>270</v>
+      <c r="D63" s="8" t="s">
+        <v>273</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>55</v>
@@ -8395,7 +8358,7 @@
       <c r="AX63" s="1"/>
       <c r="AY63" s="1"/>
       <c r="AZ63" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="BA63" s="1"/>
     </row>
@@ -8409,11 +8372,11 @@
       <c r="C64" s="1">
         <v>5.0</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>271</v>
+      <c r="D64" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>55</v>
@@ -8479,11 +8442,11 @@
       <c r="C65" s="1">
         <v>5.0</v>
       </c>
-      <c r="D65" s="9" t="s">
-        <v>272</v>
+      <c r="D65" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>55</v>
@@ -8549,11 +8512,11 @@
       <c r="C66" s="1">
         <v>5.0</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>273</v>
+      <c r="D66" s="8" t="s">
+        <v>276</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>55</v>
@@ -8619,11 +8582,11 @@
       <c r="C67" s="1">
         <v>5.0</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>274</v>
+      <c r="D67" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>55</v>
@@ -8689,11 +8652,11 @@
       <c r="C68" s="1">
         <v>5.0</v>
       </c>
-      <c r="D68" s="9" t="s">
-        <v>275</v>
+      <c r="D68" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>55</v>
@@ -8759,11 +8722,11 @@
       <c r="C69" s="1">
         <v>5.0</v>
       </c>
-      <c r="D69" s="9" t="s">
-        <v>276</v>
+      <c r="D69" s="8" t="s">
+        <v>279</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>55</v>
@@ -8830,10 +8793,10 @@
         <v>5.0</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>55</v>
@@ -8851,7 +8814,7 @@
         <v>58</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>60</v>
@@ -8863,13 +8826,13 @@
         <v>432.0</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="P70" s="1">
         <v>5.0</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R70" s="1">
         <v>1000.0</v>
@@ -8894,7 +8857,7 @@
         <v>6.0</v>
       </c>
       <c r="Z70" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AA70" s="1" t="s">
         <v>56</v>
@@ -8926,7 +8889,7 @@
       </c>
       <c r="AK70" s="1"/>
       <c r="AL70" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AM70" s="1" t="s">
         <v>58</v>
@@ -8955,19 +8918,19 @@
         <v>71</v>
       </c>
       <c r="AW70" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX70" s="2" t="s">
         <v>56</v>
       </c>
       <c r="AY70" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="AZ70" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="BA70" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB70" s="3">
         <v>45101.0</v>
@@ -8984,10 +8947,10 @@
         <v>5.0</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>55</v>
@@ -9040,7 +9003,7 @@
       <c r="AX71" s="1"/>
       <c r="AY71" s="1"/>
       <c r="AZ71" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="BA71" s="1"/>
       <c r="BB71" s="3"/>
@@ -9055,11 +9018,11 @@
       <c r="C72" s="1">
         <v>5.0</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>284</v>
+      <c r="D72" s="8" t="s">
+        <v>287</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>55</v>
@@ -9125,11 +9088,11 @@
       <c r="C73" s="1">
         <v>5.0</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>285</v>
+      <c r="D73" s="8" t="s">
+        <v>288</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>55</v>
@@ -9195,11 +9158,11 @@
       <c r="C74" s="1">
         <v>5.0</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>286</v>
+      <c r="D74" s="8" t="s">
+        <v>289</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>55</v>
@@ -9265,11 +9228,11 @@
       <c r="C75" s="1">
         <v>5.0</v>
       </c>
-      <c r="D75" s="9" t="s">
-        <v>287</v>
+      <c r="D75" s="8" t="s">
+        <v>290</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>55</v>
@@ -9335,11 +9298,11 @@
       <c r="C76" s="1">
         <v>5.0</v>
       </c>
-      <c r="D76" s="9" t="s">
-        <v>288</v>
+      <c r="D76" s="8" t="s">
+        <v>291</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>55</v>
@@ -9405,11 +9368,11 @@
       <c r="C77" s="1">
         <v>5.0</v>
       </c>
-      <c r="D77" s="9" t="s">
-        <v>289</v>
+      <c r="D77" s="8" t="s">
+        <v>292</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>55</v>
@@ -9475,11 +9438,11 @@
       <c r="C78" s="1">
         <v>5.0</v>
       </c>
-      <c r="D78" s="9" t="s">
-        <v>290</v>
+      <c r="D78" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>55</v>
@@ -9545,11 +9508,11 @@
       <c r="C79" s="1">
         <v>5.0</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>291</v>
+      <c r="D79" s="8" t="s">
+        <v>294</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>55</v>
@@ -9615,11 +9578,11 @@
       <c r="C80" s="1">
         <v>5.0</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>292</v>
+      <c r="D80" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>55</v>
@@ -9685,11 +9648,11 @@
       <c r="C81" s="1">
         <v>5.0</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>293</v>
+      <c r="D81" s="8" t="s">
+        <v>296</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>55</v>
@@ -9756,10 +9719,10 @@
         <v>5.0</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>55</v>
@@ -9826,10 +9789,10 @@
         <v>5.0</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>55</v>
@@ -9847,7 +9810,7 @@
         <v>58</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>60</v>
@@ -9859,13 +9822,13 @@
         <v>2.0</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="P83" s="1">
         <v>1.0</v>
       </c>
       <c r="Q83" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R83" s="1">
         <v>10000.0</v>
@@ -9890,7 +9853,7 @@
         <v>1.0</v>
       </c>
       <c r="Z83" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="AA83" s="1" t="s">
         <v>56</v>
@@ -9917,7 +9880,7 @@
         <v>56</v>
       </c>
       <c r="AI83" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="AJ83" s="1" t="s">
         <v>58</v>
@@ -9939,34 +9902,34 @@
         <v>56</v>
       </c>
       <c r="AQ83" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="AR83" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AS83" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="AT83" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU83" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="AV83" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AW83" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX83" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AY83" s="1" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="AZ83" s="6" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="BA83" s="1" t="s">
         <v>74</v>
@@ -9986,10 +9949,10 @@
         <v>5.0</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>55</v>
@@ -10007,21 +9970,25 @@
         <v>58</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
+        <v>309</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="N84" s="1">
         <v>33.0</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="P84" s="1">
         <v>3.0</v>
       </c>
       <c r="Q84" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R84" s="1">
         <v>5000.0</v>
@@ -10030,13 +9997,13 @@
         <v>56</v>
       </c>
       <c r="T84" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="U84" s="1" t="s">
         <v>56</v>
       </c>
       <c r="V84" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="W84" s="1" t="s">
         <v>56</v>
@@ -10048,7 +10015,7 @@
         <v>2.0</v>
       </c>
       <c r="Z84" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="AA84" s="1" t="s">
         <v>56</v>
@@ -10075,14 +10042,14 @@
         <v>56</v>
       </c>
       <c r="AI84" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="AJ84" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK84" s="1"/>
       <c r="AL84" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AM84" s="1" t="s">
         <v>58</v>
@@ -10119,7 +10086,7 @@
       <c r="AY84" s="1"/>
       <c r="AZ84" s="1"/>
       <c r="BA84" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB84" s="3">
         <v>45101.0</v>
@@ -10135,11 +10102,11 @@
       <c r="C85" s="1">
         <v>5.0</v>
       </c>
-      <c r="D85" s="9" t="s">
-        <v>310</v>
+      <c r="D85" s="8" t="s">
+        <v>313</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>55</v>
@@ -10205,11 +10172,11 @@
       <c r="C86" s="1">
         <v>5.0</v>
       </c>
-      <c r="D86" s="9" t="s">
-        <v>311</v>
+      <c r="D86" s="8" t="s">
+        <v>314</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>55</v>
@@ -10276,7 +10243,7 @@
         <v>4.0</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>54</v>
@@ -10346,7 +10313,7 @@
         <v>4.0</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>54</v>
@@ -10367,7 +10334,7 @@
         <v>58</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>60</v>
@@ -10379,13 +10346,13 @@
         <v>3.0</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="P88" s="1">
         <v>1.0</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R88" s="1">
         <v>500.0</v>
@@ -10437,7 +10404,7 @@
         <v>58</v>
       </c>
       <c r="AI88" s="1" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="AJ88" s="1" t="s">
         <v>58</v>
@@ -10465,7 +10432,7 @@
         <v>58</v>
       </c>
       <c r="AS88" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AT88" s="1" t="s">
         <v>70</v>
@@ -10482,7 +10449,7 @@
       </c>
       <c r="AY88" s="1"/>
       <c r="AZ88" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="BA88" s="1" t="s">
         <v>74</v>
@@ -10502,7 +10469,7 @@
         <v>4.0</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>54</v>
@@ -10523,10 +10490,10 @@
         <v>58</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M89" s="1" t="s">
         <v>58</v>
@@ -10535,13 +10502,13 @@
         <v>96.0</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="P89" s="1">
         <v>3.0</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R89" s="1">
         <v>1000.0</v>
@@ -10593,13 +10560,13 @@
         <v>56</v>
       </c>
       <c r="AI89" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="AJ89" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK89" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="AL89" s="1" t="s">
         <v>67</v>
@@ -10617,19 +10584,19 @@
         <v>56</v>
       </c>
       <c r="AQ89" s="2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="AR89" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AS89" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="AT89" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AU89" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="AV89" s="1" t="s">
         <v>71</v>
@@ -10641,13 +10608,13 @@
         <v>56</v>
       </c>
       <c r="AY89" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="AZ89" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BA89" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB89" s="3">
         <v>45091.0</v>
@@ -10664,7 +10631,7 @@
         <v>4.0</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>54</v>
@@ -10685,7 +10652,7 @@
         <v>58</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>60</v>
@@ -10697,13 +10664,13 @@
         <v>288.0</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="P90" s="1">
         <v>6.0</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R90" s="1">
         <v>1000.0</v>
@@ -10727,8 +10694,8 @@
       <c r="Y90" s="1">
         <v>6.0</v>
       </c>
-      <c r="Z90" s="1" t="s">
-        <v>66</v>
+      <c r="Z90" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="AA90" s="1" t="s">
         <v>56</v>
@@ -10755,13 +10722,13 @@
         <v>56</v>
       </c>
       <c r="AI90" s="1" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="AJ90" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK90" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="AL90" s="1" t="s">
         <v>67</v>
@@ -10799,13 +10766,13 @@
         <v>56</v>
       </c>
       <c r="AY90" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="AZ90" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="BA90" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB90" s="3">
         <v>45090.0</v>
@@ -10822,7 +10789,7 @@
         <v>4.0</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>54</v>
@@ -10843,7 +10810,7 @@
         <v>58</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>60</v>
@@ -10855,13 +10822,13 @@
         <v>540.0</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="P91" s="1">
         <v>5.0</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R91" s="1">
         <v>1000.0</v>
@@ -10885,8 +10852,8 @@
       <c r="Y91" s="1">
         <v>8.0</v>
       </c>
-      <c r="Z91" s="1" t="s">
-        <v>66</v>
+      <c r="Z91" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="AA91" s="1" t="s">
         <v>58</v>
@@ -10913,16 +10880,16 @@
         <v>56</v>
       </c>
       <c r="AI91" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="AJ91" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK91" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="AL91" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="AM91" s="1" t="s">
         <v>58</v>
@@ -10937,7 +10904,7 @@
         <v>56</v>
       </c>
       <c r="AQ91" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="AR91" s="1" t="s">
         <v>56</v>
@@ -10951,19 +10918,19 @@
         <v>71</v>
       </c>
       <c r="AW91" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX91" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AY91" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="AZ91" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="BA91" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB91" s="3">
         <v>45092.0</v>
@@ -10980,7 +10947,7 @@
         <v>4.0</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>54</v>
@@ -11001,7 +10968,7 @@
         <v>58</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>60</v>
@@ -11013,13 +10980,13 @@
         <v>18.0</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="P92" s="1">
         <v>3.0</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R92" s="1">
         <v>1000.0</v>
@@ -11071,15 +11038,17 @@
         <v>58</v>
       </c>
       <c r="AI92" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="AJ92" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK92" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="AL92" s="1"/>
+        <v>351</v>
+      </c>
+      <c r="AL92" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="AM92" s="1" t="s">
         <v>58</v>
       </c>
@@ -11099,7 +11068,7 @@
         <v>58</v>
       </c>
       <c r="AS92" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="AT92" s="1" t="s">
         <v>70</v>
@@ -11109,17 +11078,17 @@
         <v>71</v>
       </c>
       <c r="AW92" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX92" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AY92" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="AZ92" s="1"/>
       <c r="BA92" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BB92" s="3">
         <v>45092.0</v>
@@ -11136,7 +11105,7 @@
         <v>4.0</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>54</v>
@@ -11157,10 +11126,10 @@
         <v>58</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M93" s="1" t="s">
         <v>58</v>
@@ -11169,13 +11138,13 @@
         <v>2.0</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="P93" s="1">
         <v>1.0</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R93" s="1">
         <v>10000.0</v>
@@ -11184,7 +11153,7 @@
         <v>56</v>
       </c>
       <c r="T93" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="U93" s="1" t="s">
         <v>58</v>
@@ -11202,7 +11171,7 @@
         <v>9.0</v>
       </c>
       <c r="Z93" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="AA93" s="1" t="s">
         <v>56</v>
@@ -11229,16 +11198,16 @@
         <v>56</v>
       </c>
       <c r="AI93" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="AJ93" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK93" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="AL93" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="AM93" s="1" t="s">
         <v>56</v>
@@ -11273,13 +11242,13 @@
         <v>56</v>
       </c>
       <c r="AY93" s="1" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="AZ93" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="BA93" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB93" s="3">
         <v>45095.0</v>
@@ -11296,7 +11265,7 @@
         <v>4.0</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>54</v>
@@ -11317,10 +11286,10 @@
         <v>58</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M94" s="1" t="s">
         <v>58</v>
@@ -11329,7 +11298,7 @@
         <v>15.0</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="P94" s="1">
         <v>4.0</v>
@@ -11413,7 +11382,7 @@
         <v>58</v>
       </c>
       <c r="AS94" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="AT94" s="1" t="s">
         <v>70</v>
@@ -11423,17 +11392,17 @@
         <v>71</v>
       </c>
       <c r="AW94" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX94" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AY94" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="AZ94" s="1"/>
       <c r="BA94" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB94" s="3">
         <v>45095.0</v>
@@ -11450,7 +11419,7 @@
         <v>4.0</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>54</v>
@@ -11471,7 +11440,7 @@
         <v>58</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>60</v>
@@ -11483,13 +11452,13 @@
         <v>81.0</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="P95" s="1">
         <v>4.0</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R95" s="1">
         <v>10.0</v>
@@ -11541,14 +11510,14 @@
         <v>56</v>
       </c>
       <c r="AI95" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="AJ95" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK95" s="1"/>
       <c r="AL95" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="AM95" s="1" t="s">
         <v>58</v>
@@ -11583,13 +11552,13 @@
         <v>56</v>
       </c>
       <c r="AY95" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="AZ95" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="BA95" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB95" s="3">
         <v>45095.0</v>
@@ -11606,10 +11575,10 @@
         <v>3.0</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F96" s="13" t="s">
         <v>55</v>
@@ -11627,7 +11596,7 @@
         <v>58</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="L96" s="13" t="s">
         <v>60</v>
@@ -11639,13 +11608,13 @@
         <v>4.0</v>
       </c>
       <c r="O96" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P96" s="11">
         <v>1.0</v>
       </c>
       <c r="Q96" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R96" s="11">
         <v>1000.0</v>
@@ -11697,13 +11666,13 @@
         <v>56</v>
       </c>
       <c r="AI96" s="15" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="AJ96" s="15" t="s">
         <v>58</v>
       </c>
       <c r="AK96" s="15" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="AL96" s="15" t="s">
         <v>67</v>
@@ -11721,13 +11690,13 @@
         <v>56</v>
       </c>
       <c r="AQ96" s="13" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="AR96" s="13" t="s">
         <v>58</v>
       </c>
       <c r="AS96" s="13" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="AT96" s="13" t="s">
         <v>70</v>
@@ -11737,16 +11706,16 @@
         <v>71</v>
       </c>
       <c r="AW96" s="13" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX96" s="13" t="s">
         <v>56</v>
       </c>
       <c r="AY96" s="13" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="BA96" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB96" s="16">
         <v>45145.0</v>
@@ -11754,7 +11723,7 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="17" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B97" s="2">
         <v>2022.0</v>
@@ -11763,10 +11732,10 @@
         <v>1.0</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>55</v>
@@ -11784,7 +11753,7 @@
         <v>58</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="L97" s="1" t="s">
         <v>60</v>
@@ -11796,7 +11765,7 @@
         <v>216.0</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="P97" s="1">
         <v>6.0</v>
@@ -11815,7 +11784,7 @@
         <v>64</v>
       </c>
       <c r="V97" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="W97" s="1" t="s">
         <v>58</v>
@@ -11854,16 +11823,16 @@
         <v>56</v>
       </c>
       <c r="AI97" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="AJ97" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK97" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="AL97" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="AM97" s="1" t="s">
         <v>58</v>
@@ -11884,31 +11853,31 @@
         <v>58</v>
       </c>
       <c r="AS97" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="AT97" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU97" s="5" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="AV97" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AW97" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX97" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AY97" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="AZ97" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="BA97" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB97" s="3">
         <v>45109.0</v>
@@ -11916,7 +11885,7 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="17" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B98" s="2">
         <v>2022.0</v>
@@ -11925,7 +11894,7 @@
         <v>6.0</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>54</v>
@@ -11946,7 +11915,7 @@
         <v>58</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="L98" s="1" t="s">
         <v>60</v>
@@ -11958,13 +11927,13 @@
         <v>3.0</v>
       </c>
       <c r="O98" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P98" s="1">
         <v>1.0</v>
       </c>
       <c r="Q98" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R98" s="1">
         <v>30.0</v>
@@ -11977,7 +11946,7 @@
         <v>64</v>
       </c>
       <c r="V98" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="W98" s="1" t="s">
         <v>58</v>
@@ -11988,8 +11957,8 @@
       <c r="Y98" s="1">
         <v>2.0</v>
       </c>
-      <c r="Z98" s="1" t="s">
-        <v>66</v>
+      <c r="Z98" s="2" t="s">
+        <v>397</v>
       </c>
       <c r="AA98" s="1" t="s">
         <v>56</v>
@@ -12016,14 +11985,14 @@
         <v>56</v>
       </c>
       <c r="AI98" s="1" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="AJ98" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK98" s="1"/>
       <c r="AL98" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM98" s="1" t="s">
         <v>56</v>
@@ -12038,37 +12007,37 @@
         <v>56</v>
       </c>
       <c r="AQ98" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AR98" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AS98" s="1" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="AT98" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AU98" s="1" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="AV98" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AW98" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="AX98" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AY98" s="1" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="AZ98" s="1" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="BA98" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB98" s="3">
         <v>45109.0</v>
@@ -12076,7 +12045,7 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="17" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B99" s="2">
         <v>2022.0</v>
@@ -12085,10 +12054,10 @@
         <v>1.0</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>55</v>
@@ -12106,10 +12075,10 @@
         <v>58</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M99" s="1" t="s">
         <v>58</v>
@@ -12118,13 +12087,13 @@
         <v>3.0</v>
       </c>
       <c r="O99" s="1" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="P99" s="1">
         <v>1.0</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R99" s="1">
         <v>1.0</v>
@@ -12176,13 +12145,13 @@
         <v>56</v>
       </c>
       <c r="AI99" s="1" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="AJ99" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AK99" s="1" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="AL99" s="1" t="s">
         <v>67</v>
@@ -12200,7 +12169,7 @@
         <v>56</v>
       </c>
       <c r="AQ99" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="AR99" s="1" t="s">
         <v>56</v>
@@ -12220,11 +12189,11 @@
         <v>56</v>
       </c>
       <c r="AY99" s="1" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="AZ99" s="1"/>
       <c r="BA99" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB99" s="3">
         <v>45109.0</v>
@@ -12232,7 +12201,7 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="17" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B100" s="2">
         <v>2022.0</v>
@@ -12241,10 +12210,10 @@
         <v>3.0</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>55</v>
@@ -12262,7 +12231,7 @@
         <v>58</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="L100" s="1" t="s">
         <v>60</v>
@@ -12274,13 +12243,13 @@
         <v>8.0</v>
       </c>
       <c r="O100" s="1" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="P100" s="1">
         <v>3.0</v>
       </c>
       <c r="Q100" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R100" s="1">
         <v>20.0</v>
@@ -12293,7 +12262,7 @@
         <v>64</v>
       </c>
       <c r="V100" s="1" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="W100" s="1" t="s">
         <v>58</v>
@@ -12332,13 +12301,13 @@
         <v>56</v>
       </c>
       <c r="AI100" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="AJ100" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AL100" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AM100" s="1" t="s">
         <v>58</v>
@@ -12359,7 +12328,7 @@
         <v>58</v>
       </c>
       <c r="AS100" s="1" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="AT100" s="1" t="s">
         <v>70</v>
@@ -12372,10 +12341,10 @@
         <v>72</v>
       </c>
       <c r="AX100" s="1" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="AY100" s="1" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="AZ100" s="1"/>
       <c r="BA100" s="1" t="s">
@@ -12387,7 +12356,7 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="17" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B101" s="2">
         <v>2022.0</v>
@@ -12396,7 +12365,7 @@
         <v>44987.0</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>54</v>
@@ -12417,7 +12386,7 @@
         <v>58</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="L101" s="1" t="s">
         <v>60</v>
@@ -12429,13 +12398,13 @@
         <v>135.0</v>
       </c>
       <c r="O101" s="1" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="P101" s="1">
         <v>4.0</v>
       </c>
       <c r="Q101" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R101" s="1">
         <v>5000.0</v>
@@ -12459,8 +12428,8 @@
       <c r="Y101" s="1">
         <v>1.0</v>
       </c>
-      <c r="Z101" s="1" t="s">
-        <v>215</v>
+      <c r="Z101" s="2" t="s">
+        <v>420</v>
       </c>
       <c r="AA101" s="1" t="s">
         <v>56</v>
@@ -12487,16 +12456,16 @@
         <v>56</v>
       </c>
       <c r="AI101" s="1" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="AJ101" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AK101" s="1" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="AL101" s="1" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="AM101" s="1" t="s">
         <v>58</v>
@@ -12531,11 +12500,11 @@
         <v>56</v>
       </c>
       <c r="AY101" s="1" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="AZ101" s="1"/>
       <c r="BA101" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB101" s="3">
         <v>45110.0</v>
@@ -12543,7 +12512,7 @@
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="17" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B102" s="2">
         <v>2022.0</v>
@@ -12552,10 +12521,10 @@
         <v>4.0</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>55</v>
@@ -12573,9 +12542,11 @@
         <v>58</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="L102" s="1"/>
+        <v>426</v>
+      </c>
+      <c r="L102" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="M102" s="1" t="s">
         <v>58</v>
       </c>
@@ -12583,13 +12554,13 @@
         <v>72.0</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="P102" s="1">
         <v>5.0</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R102" s="1">
         <v>5000.0</v>
@@ -12613,8 +12584,8 @@
       <c r="Y102" s="1">
         <v>6.0</v>
       </c>
-      <c r="Z102" s="1" t="s">
-        <v>66</v>
+      <c r="Z102" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="AA102" s="1" t="s">
         <v>58</v>
@@ -12645,7 +12616,7 @@
         <v>58</v>
       </c>
       <c r="AK102" s="1" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="AL102" s="1"/>
       <c r="AM102" s="1" t="s">
@@ -12661,19 +12632,19 @@
         <v>56</v>
       </c>
       <c r="AQ102" s="2" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="AR102" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AS102" s="1" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="AT102" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU102" s="1" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="AV102" s="1" t="s">
         <v>58</v>
@@ -12685,11 +12656,11 @@
         <v>56</v>
       </c>
       <c r="AY102" s="1" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="AZ102" s="1"/>
       <c r="BA102" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB102" s="3">
         <v>45110.0</v>
@@ -17825,89 +17796,92 @@
     <mergeCell ref="AY96:AZ96"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ25">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,Ox"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ97">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,SPSS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ102">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,R, Mplus, OpenMX"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X2:X149">
+      <formula1>"known,estimated"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ2:AQ4 AQ6:AQ10 AQ12:AQ17 AQ19:AQ24 AQ26:AQ28 AQ30:AQ49 AQ51:AQ54 AQ56:AQ82 AQ84:AQ88 AQ90 AQ92:AQ93 AQ95 AQ99:AQ101 AQ103:AQ149">
+      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q2:Q149">
+      <formula1>"fully-factorial,partially-factorial,one-at-a-time"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ11">
+      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear,R, Stata"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ50">
       <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,SAS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L3 L5:L149">
-      <formula1>"resampled,parametric based on actual data,parametric thin-air"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Z5">
+      <formula1>"estimation,testing,model selection,prediction,design,other,estimation, model selection"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ91">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,MATLAB, R"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Z2:Z4 Z6:Z149">
+      <formula1>"estimation,testing,model selection,prediction,design,other,estimation, model selection,design, estimation,estimation, testing,estimation, testing,estimation, classification,model selection, testing,estimation, testing"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ29">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,R, Mplus"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ5">
+      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear,R, Stan"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ18 AQ98">
+      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear,R, JAGS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ94">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,R, Stan"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AT2:AT149">
+      <formula1>"accessible online,not accessible"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ89">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,SAS, Mplus"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G149">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BA2:BA149">
+      <formula1>"great,medium,poor"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E149">
+      <formula1>"BRM,PM,MBRM"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ25">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,Ox"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ96">
       <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,R, MATLAB"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ91">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,MATLAB, R"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J3 M2:M3 J5:J149 M5:M149 S2:S149 U2:U149 W2:W149 AA2:AH149 AJ2:AJ149 AM2:AP149 AR2:AR149">
+      <formula1>"yes,no,unclear"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E149">
-      <formula1>"BRM,PM,MBRM"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L3 L5:L149">
+      <formula1>"resampled,parametric based on actual data,parametric thin-air"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ94">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,R, Stan"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AW2:AW149">
+      <formula1>"fully,partially,minimal,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BA2:BA149">
-      <formula1>"great,medium,poor"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q2:Q149">
-      <formula1>"fully-factorial,partially-factorial,one-at-a-time"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ55">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,JAGS"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F149">
       <formula1>"SP,FB,BS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ11">
-      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear,R, Stata"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AT2:AT149">
-      <formula1>"accessible online,not accessible"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G149">
-      <formula1>"yes,no"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ83">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,C++, Python"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Z2:Z149">
-      <formula1>"estimation,testing,model selection,prediction,design,other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ55">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,JAGS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ2:AQ4 AQ6:AQ10 AQ12:AQ17 AQ19:AQ24 AQ26:AQ28 AQ30:AQ49 AQ51:AQ54 AQ56:AQ82 AQ84:AQ88 AQ90 AQ92:AQ93 AQ95 AQ99:AQ101 AQ103:AQ149">
-      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ18 AQ98">
-      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear,R, JAGS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ102">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,R, Mplus, OpenMX"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AV2:AV149">
       <formula1>"yes,not found"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ89">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,SAS, Mplus"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ5">
-      <formula1>"R,MATLAB,Python,Stata,Excel,R,Mplus,unclear,R, Stan"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J3 M2:M3 J5:J149 M5:M149 S2:S149 U2:U149 W2:W149 AA2:AH149 AJ2:AJ149 AM2:AP149 AR2:AR149">
-      <formula1>"yes,no,unclear"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AX2:AX149">
       <formula1>"fully,partially,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X2:X149">
-      <formula1>"known,estimated"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ97">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,SPSS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ29">
-      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,R, Mplus"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AW2:AW149">
-      <formula1>"fully,partially,minimal,no"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AQ83">
+      <formula1>"R,MATLAB,Python,Stata,Excel,Mplus,unclear,C++, Python"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>